<commit_message>
Included the split of eroded phase space
</commit_message>
<xml_diff>
--- a/Setup/MazeDimensions_new2021_ant.xlsx
+++ b/Setup/MazeDimensions_new2021_ant.xlsx
@@ -107,21 +107,12 @@
     <t>arena_height</t>
   </si>
   <si>
-    <t>23, 29.714</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
     <t>arena_length</t>
   </si>
   <si>
-    <t>15.3, 17.739</t>
-  </si>
-  <si>
-    <t>13.8, 17.3</t>
-  </si>
-  <si>
     <t>L_LASH</t>
   </si>
   <si>
@@ -156,6 +147,15 @@
   </si>
   <si>
     <t>2.65, 3.42</t>
+  </si>
+  <si>
+    <t>3.28, 4.77</t>
+  </si>
+  <si>
+    <t>6.56, 9.51</t>
+  </si>
+  <si>
+    <t>13.12, 19.02</t>
   </si>
 </sst>
 </file>
@@ -476,7 +476,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,10 +490,10 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
         <v>28</v>
-      </c>
-      <c r="B1" t="s">
-        <v>29</v>
       </c>
       <c r="C1" t="s">
         <v>26</v>
@@ -516,16 +516,16 @@
         <v>40</v>
       </c>
       <c r="C2">
-        <v>17.5</v>
+        <v>19.190000000000001</v>
       </c>
       <c r="D2">
         <v>3.7</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="F2">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -533,19 +533,19 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>9.6</v>
       </c>
       <c r="D3">
         <v>1.85</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="F3">
-        <v>0.2</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -553,19 +553,19 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C4">
-        <v>9.92</v>
+        <v>4.8</v>
       </c>
       <c r="D4">
-        <v>0.92500000000000004</v>
+        <v>0.92</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="F4">
-        <v>0.13</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -582,7 +582,7 @@
         <v>0.54</v>
       </c>
       <c r="E5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F5">
         <v>0.08</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B18">
         <v>35.200000000000003</v>
@@ -975,7 +975,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>35.200000000000003</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>35.200000000000003</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B35">
         <v>35.200000000000003</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B36">
         <v>35.200000000000003</v>
@@ -1055,7 +1055,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B37">
         <v>35.200000000000003</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B38">
         <v>35.200000000000003</v>
@@ -1095,7 +1095,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B39">
         <v>35.200000000000003</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B40">
         <v>35.200000000000003</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B41">
         <v>35.200000000000003</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B42">
         <v>35.200000000000003</v>

</xml_diff>

<commit_message>
Made dilation and erosion static methods.
</commit_message>
<xml_diff>
--- a/Setup/MazeDimensions_new2021_ant.xlsx
+++ b/Setup/MazeDimensions_new2021_ant.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27768" windowHeight="12528"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27765" windowHeight="12525"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
     <t>6.56, 9.51</t>
   </si>
   <si>
-    <t>13.12, 19.02</t>
+    <t>13.12, 18.6</t>
   </si>
 </sst>
 </file>
@@ -476,19 +476,19 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -508,7 +508,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -528,7 +528,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -548,7 +548,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -568,7 +568,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -588,7 +588,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -608,7 +608,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -628,7 +628,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -648,7 +648,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -668,7 +668,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -688,7 +688,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -708,7 +708,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -728,7 +728,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -748,7 +748,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -768,7 +768,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -788,7 +788,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -808,7 +808,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -828,7 +828,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -848,7 +848,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -868,7 +868,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -888,7 +888,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -908,7 +908,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -928,7 +928,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -948,7 +948,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -968,12 +968,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -993,7 +993,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1033,7 +1033,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1093,7 +1093,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1133,7 +1133,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
I decreased the wall thickness by an eigth. Because I think, that the non-rounded edges of the SPT in the PhysicsEngine ot impossible to solve otherwise.
</commit_message>
<xml_diff>
--- a/Setup/MazeDimensions_new2021_ant.xlsx
+++ b/Setup/MazeDimensions_new2021_ant.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabea\PycharmProjects\AntsShapes\Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421F2DEC-FC25-4B5F-8A53-475F33F8467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27765" windowHeight="12525"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t>exit_size</t>
   </si>
@@ -156,12 +157,15 @@
   </si>
   <si>
     <t>13.12, 18.6</t>
+  </si>
+  <si>
+    <t>measured</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -472,23 +476,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.26953125" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -507,8 +511,11 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -525,10 +532,28 @@
         <v>43</v>
       </c>
       <c r="F2">
+        <v>0.35</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <v>19.190000000000001</v>
+      </c>
+      <c r="K2">
+        <v>3.7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M2">
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -545,10 +570,28 @@
         <v>42</v>
       </c>
       <c r="F3">
+        <v>0.25</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>9.6</v>
+      </c>
+      <c r="K3">
+        <v>1.85</v>
+      </c>
+      <c r="L3" t="s">
+        <v>42</v>
+      </c>
+      <c r="M3">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -565,10 +608,28 @@
         <v>41</v>
       </c>
       <c r="F4">
+        <v>0.12</v>
+      </c>
+      <c r="H4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <v>4.8</v>
+      </c>
+      <c r="K4">
+        <v>0.92</v>
+      </c>
+      <c r="L4" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4">
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -585,10 +646,28 @@
         <v>40</v>
       </c>
       <c r="F5">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
+      </c>
+      <c r="J5">
+        <v>2.48</v>
+      </c>
+      <c r="K5">
+        <v>0.54</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5">
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -608,7 +687,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -628,7 +707,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -648,7 +727,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -668,7 +747,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -688,7 +767,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -708,7 +787,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -728,7 +807,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -748,7 +827,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -768,7 +847,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -788,7 +867,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -808,7 +887,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -828,7 +907,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -848,7 +927,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -868,7 +947,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -888,7 +967,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -908,7 +987,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -928,7 +1007,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -948,7 +1027,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -968,12 +1047,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -993,7 +1072,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1013,7 +1092,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1033,7 +1112,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1053,7 +1132,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1073,7 +1152,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1093,7 +1172,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1113,7 +1192,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1133,7 +1212,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1153,7 +1232,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
I added a functionality, that only part of the PhaseSpace will be calculated.
</commit_message>
<xml_diff>
--- a/Setup/MazeDimensions_new2021_ant.xlsx
+++ b/Setup/MazeDimensions_new2021_ant.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tabea\PycharmProjects\AntsShapes\Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{421F2DEC-FC25-4B5F-8A53-475F33F8467E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>exit_size</t>
   </si>
@@ -160,12 +159,24 @@
   </si>
   <si>
     <t>measured</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.12</t>
+  </si>
+  <si>
+    <t>0.07</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,23 +487,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="20.453125" customWidth="1"/>
-    <col min="3" max="3" width="21.26953125" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="18.54296875" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
@@ -515,7 +526,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -531,8 +542,8 @@
       <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="F2">
-        <v>0.35</v>
+      <c r="F2" t="s">
+        <v>45</v>
       </c>
       <c r="H2" t="s">
         <v>3</v>
@@ -553,7 +564,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -569,8 +580,8 @@
       <c r="E3" t="s">
         <v>42</v>
       </c>
-      <c r="F3">
-        <v>0.25</v>
+      <c r="F3" t="s">
+        <v>46</v>
       </c>
       <c r="H3" t="s">
         <v>4</v>
@@ -591,7 +602,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -607,8 +618,8 @@
       <c r="E4" t="s">
         <v>41</v>
       </c>
-      <c r="F4">
-        <v>0.12</v>
+      <c r="F4" t="s">
+        <v>47</v>
       </c>
       <c r="H4" t="s">
         <v>5</v>
@@ -629,7 +640,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -645,8 +656,8 @@
       <c r="E5" t="s">
         <v>40</v>
       </c>
-      <c r="F5">
-        <v>7.0000000000000007E-2</v>
+      <c r="F5" t="s">
+        <v>48</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
@@ -667,7 +678,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -687,7 +698,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -707,7 +718,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -727,7 +738,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -747,7 +758,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -767,7 +778,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -787,7 +798,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -807,7 +818,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -827,7 +838,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -847,7 +858,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -867,7 +878,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -887,7 +898,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -907,7 +918,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -927,7 +938,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>19</v>
       </c>
@@ -947,7 +958,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>20</v>
       </c>
@@ -967,7 +978,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -987,7 +998,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1007,7 +1018,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1027,7 +1038,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -1047,12 +1058,12 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1072,7 +1083,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1092,7 +1103,7 @@
         <v>0.40600000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -1112,7 +1123,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>39</v>
       </c>
@@ -1132,7 +1143,7 @@
         <v>0.30449999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>29</v>
       </c>
@@ -1152,7 +1163,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -1172,7 +1183,7 @@
         <v>0.20300000000000001</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>31</v>
       </c>
@@ -1192,7 +1203,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>32</v>
       </c>
@@ -1212,7 +1223,7 @@
         <v>0.10150000000000001</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>33</v>
       </c>
@@ -1232,7 +1243,7 @@
         <v>5.0750000000000003E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>34</v>
       </c>

</xml_diff>